<commit_message>
Jackie - add date to timesheet
</commit_message>
<xml_diff>
--- a/01.documentation/timesheet/jackie-timesheet.xlsx
+++ b/01.documentation/timesheet/jackie-timesheet.xlsx
@@ -497,7 +497,7 @@
   <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -637,6 +637,9 @@
       <c r="A13" t="s">
         <v>14</v>
       </c>
+      <c r="B13" s="1">
+        <v>41721</v>
+      </c>
       <c r="C13">
         <v>2.5</v>
       </c>
@@ -645,6 +648,9 @@
       <c r="A14" t="s">
         <v>15</v>
       </c>
+      <c r="B14" s="1">
+        <v>41721</v>
+      </c>
       <c r="C14">
         <v>1</v>
       </c>
@@ -653,6 +659,9 @@
       <c r="A15" t="s">
         <v>15</v>
       </c>
+      <c r="B15" s="1">
+        <v>41723</v>
+      </c>
       <c r="C15">
         <v>5</v>
       </c>
@@ -660,6 +669,9 @@
     <row r="16" spans="1:3">
       <c r="A16" t="s">
         <v>16</v>
+      </c>
+      <c r="B16" s="1">
+        <v>41724</v>
       </c>
       <c r="C16">
         <v>1</v>

</xml_diff>

<commit_message>
Jackie - update timesheet
</commit_message>
<xml_diff>
--- a/01.documentation/timesheet/jackie-timesheet.xlsx
+++ b/01.documentation/timesheet/jackie-timesheet.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
   <si>
     <t>Description</t>
   </si>
@@ -72,55 +72,58 @@
     <t>Discuss with the team, Make Chnages base on the team's suggestion</t>
   </si>
   <si>
-    <t>Design the Master Page</t>
-  </si>
-  <si>
     <t>Meeting with Claudia and Reshma about the Master Page</t>
   </si>
   <si>
-    <t>Develop main navigation development</t>
-  </si>
-  <si>
-    <t>Develop program pages</t>
-  </si>
-  <si>
     <t>Meeting on Google hangout with Claudia and Reshma and discuss the next move</t>
   </si>
   <si>
     <t>Discuss with Reshma about the problem with program pages</t>
   </si>
   <si>
-    <t>Work on details page</t>
-  </si>
-  <si>
     <t>Discuss with Claudia about her meeting with Reshma &amp; Bernie &amp; Jonna</t>
   </si>
   <si>
-    <t>Create lightbox gallery</t>
-  </si>
-  <si>
     <t>Go over isotope with Claudia on the phone</t>
   </si>
   <si>
     <t>Meeting with Reshma and Claudia about next step</t>
   </si>
   <si>
-    <t>Update header &amp; footer</t>
-  </si>
-  <si>
     <t>Update main nav</t>
   </si>
   <si>
     <t>Create about page design</t>
   </si>
   <si>
-    <t>develop about page</t>
-  </si>
-  <si>
     <t>Fix background-image position</t>
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Develop main navigation development and Responsive Design</t>
+  </si>
+  <si>
+    <t>Develop program pages and make it Responsive</t>
+  </si>
+  <si>
+    <t>Work on details page and make responsive design</t>
+  </si>
+  <si>
+    <t>Create lightbox gallery and Resposnvie design</t>
+  </si>
+  <si>
+    <t>Update header &amp; footer and make it respsive</t>
+  </si>
+  <si>
+    <t>develop about page and make it Responsive</t>
+  </si>
+  <si>
+    <t>Responsive Design for Splash</t>
+  </si>
+  <si>
+    <t>Research for inspiration &amp; Design the Master Page &amp; Responsive design</t>
   </si>
 </sst>
 </file>
@@ -494,10 +497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -556,7 +559,7 @@
         <v>41697</v>
       </c>
       <c r="C5">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -575,7 +578,7 @@
         <v>6</v>
       </c>
       <c r="C7">
-        <v>0.25</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -668,10 +671,10 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="B16" s="1">
-        <v>41724</v>
+        <v>41723</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -679,29 +682,29 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" s="1">
-        <v>41746</v>
+        <v>41724</v>
       </c>
       <c r="C17">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="B18" s="1">
-        <v>41750</v>
+        <v>41746</v>
       </c>
       <c r="C18">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B19" s="1">
         <v>41750</v>
@@ -712,134 +715,134 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B20" s="1">
-        <v>41755</v>
+        <v>41750</v>
       </c>
       <c r="C20">
-        <v>2.5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="B21" s="1">
-        <v>41757</v>
+        <v>41755</v>
       </c>
       <c r="C21">
-        <v>1.75</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B22" s="1">
         <v>41757</v>
       </c>
       <c r="C22">
-        <v>0.5</v>
+        <v>1.75</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B23" s="1">
-        <v>41758</v>
+        <v>41757</v>
       </c>
       <c r="C23">
-        <v>2</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B24" s="1">
-        <v>41759</v>
+        <v>41758</v>
       </c>
       <c r="C24">
-        <v>1</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="B25" s="1">
-        <v>41760</v>
+        <v>41759</v>
       </c>
       <c r="C25">
-        <v>1</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B26" s="1">
         <v>41760</v>
       </c>
       <c r="C26">
-        <v>0.25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B27" s="1">
         <v>41760</v>
       </c>
       <c r="C27">
-        <v>1.5</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B28" s="1">
         <v>41760</v>
       </c>
       <c r="C28">
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B29" s="1">
         <v>41760</v>
       </c>
       <c r="C29">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B30" s="1">
-        <v>41761</v>
+        <v>41760</v>
       </c>
       <c r="C30">
-        <v>1</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B31" s="1">
-        <v>41763</v>
+        <v>41761</v>
       </c>
       <c r="C31">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -847,19 +850,30 @@
         <v>32</v>
       </c>
       <c r="B32" s="1">
+        <v>41763</v>
+      </c>
+      <c r="C32">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" t="s">
+        <v>25</v>
+      </c>
+      <c r="B33" s="1">
         <v>41765</v>
       </c>
-      <c r="C32">
+      <c r="C33">
         <v>0.25</v>
       </c>
     </row>
-    <row r="33" spans="2:3">
-      <c r="B33" t="s">
-        <v>33</v>
-      </c>
-      <c r="C33">
-        <f>SUM(C2:C32)</f>
-        <v>38.25</v>
+    <row r="34" spans="1:3">
+      <c r="B34" t="s">
+        <v>26</v>
+      </c>
+      <c r="C34">
+        <f>SUM(C2:C33)</f>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Jackie - update again
</commit_message>
<xml_diff>
--- a/01.documentation/timesheet/jackie-timesheet.xlsx
+++ b/01.documentation/timesheet/jackie-timesheet.xlsx
@@ -42,9 +42,6 @@
     <t>Finalized moodboard</t>
   </si>
   <si>
-    <t>Research for inspiration</t>
-  </si>
-  <si>
     <t>Discuss Brnading &amp; moodboard &amp; Typography with Claudia</t>
   </si>
   <si>
@@ -124,6 +121,9 @@
   </si>
   <si>
     <t>Research for inspiration &amp; Design the Master Page &amp; Responsive design</t>
+  </si>
+  <si>
+    <t>Research for inspiration &amp; plugins</t>
   </si>
 </sst>
 </file>
@@ -500,7 +500,7 @@
   <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -522,7 +522,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" s="2">
         <v>41695</v>
@@ -533,11 +533,11 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -564,7 +564,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" s="1">
         <v>41698</v>
@@ -594,7 +594,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" s="1">
         <v>41701</v>
@@ -605,7 +605,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" s="1">
         <v>41703</v>
@@ -616,7 +616,7 @@
     </row>
     <row r="11" spans="1:3" ht="30">
       <c r="A11" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11" s="1">
         <v>41705</v>
@@ -627,7 +627,7 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12" s="1">
         <v>41717</v>
@@ -638,7 +638,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13" s="1">
         <v>41721</v>
@@ -649,7 +649,7 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14" s="1">
         <v>41721</v>
@@ -660,7 +660,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" s="1">
         <v>41723</v>
@@ -671,7 +671,7 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B16" s="1">
         <v>41723</v>
@@ -682,7 +682,7 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" s="1">
         <v>41724</v>
@@ -693,7 +693,7 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B18" s="1">
         <v>41746</v>
@@ -704,7 +704,7 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B19" s="1">
         <v>41750</v>
@@ -715,7 +715,7 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B20" s="1">
         <v>41750</v>
@@ -726,7 +726,7 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B21" s="1">
         <v>41755</v>
@@ -737,7 +737,7 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B22" s="1">
         <v>41757</v>
@@ -748,7 +748,7 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B23" s="1">
         <v>41757</v>
@@ -759,7 +759,7 @@
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B24" s="1">
         <v>41758</v>
@@ -770,7 +770,7 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B25" s="1">
         <v>41759</v>
@@ -781,7 +781,7 @@
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B26" s="1">
         <v>41760</v>
@@ -792,7 +792,7 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B27" s="1">
         <v>41760</v>
@@ -803,7 +803,7 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B28" s="1">
         <v>41760</v>
@@ -814,7 +814,7 @@
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B29" s="1">
         <v>41760</v>
@@ -825,7 +825,7 @@
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B30" s="1">
         <v>41760</v>
@@ -836,7 +836,7 @@
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B31" s="1">
         <v>41761</v>
@@ -847,7 +847,7 @@
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B32" s="1">
         <v>41763</v>
@@ -858,7 +858,7 @@
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B33" s="1">
         <v>41765</v>
@@ -869,11 +869,11 @@
     </row>
     <row r="34" spans="1:3">
       <c r="B34" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C34">
         <f>SUM(C2:C33)</f>
-        <v>58</v>
+        <v>58.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>